<commit_message>
Menü umgebaut, Kleine Nacharbeiten notwendig
* Das Menü wurde komplett überarbeitet
* Eingige Buttons sind umgezogen (direkt ins neue Menü)
* Ein paar Buttons fehlen noch (s. Übersicht Buttons)
</commit_message>
<xml_diff>
--- a/Docs/Übersicht Buttons.xlsx
+++ b/Docs/Übersicht Buttons.xlsx
@@ -198,9 +198,6 @@
     <t>Inputbutton mit Bild</t>
   </si>
   <si>
-    <t>././Bilder/Tagebuch.png</t>
-  </si>
-  <si>
     <t>Verwendung alt</t>
   </si>
   <si>
@@ -210,15 +207,9 @@
     <t>Ausruhen</t>
   </si>
   <si>
-    <t>././Bilder/weltkarte.png</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>././Bilder/ausruhen.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Speichern </t>
   </si>
   <si>
@@ -228,15 +219,9 @@
     <t>Handwerk</t>
   </si>
   <si>
-    <t>././Bilder/Handwerk.png</t>
-  </si>
-  <si>
     <t>Gepäck betrachten</t>
   </si>
   <si>
-    <t>././Bilder/gepaeckbutton.png</t>
-  </si>
-  <si>
     <t>Essen</t>
   </si>
   <si>
@@ -249,9 +234,6 @@
     <t>Gebiet erkunden</t>
   </si>
   <si>
-    <t>././Bilder/erkundenbutton.png</t>
-  </si>
-  <si>
     <t>Normale Erkundung</t>
   </si>
   <si>
@@ -267,15 +249,9 @@
     <t>Fliegen</t>
   </si>
   <si>
-    <t>././Bilder/flugbutton.png</t>
-  </si>
-  <si>
     <t>Drachenkampf</t>
   </si>
   <si>
-    <t>././Bilder/drachenkampf.png</t>
-  </si>
-  <si>
     <t>Aktion beenden</t>
   </si>
   <si>
@@ -300,12 +276,6 @@
     <t>Gefundene Dinge ignorieren</t>
   </si>
   <si>
-    <t>././Bilder/jagenbutton.png</t>
-  </si>
-  <si>
-    <t>././Bilder/pflanzenbutton.png</t>
-  </si>
-  <si>
     <t>ansprechen</t>
   </si>
   <si>
@@ -315,9 +285,6 @@
     <t>Elemente beschwören</t>
   </si>
   <si>
-    <t>././Bilder/elementbutton.png</t>
-  </si>
-  <si>
     <t>Elemente der Luft</t>
   </si>
   <si>
@@ -327,24 +294,9 @@
     <t>Elemente des Feuers</t>
   </si>
   <si>
-    <t>././Bilder/luftelemente.png</t>
-  </si>
-  <si>
-    <t>././Bilder/wasserelemente.png</t>
-  </si>
-  <si>
-    <t>././Bilder/feuerelemente.png</t>
-  </si>
-  <si>
     <t>Elemente der Erde</t>
   </si>
   <si>
-    <t>././Bilder/erdelemente.png</t>
-  </si>
-  <si>
-    <t>././Bilder/standardangriffe.png</t>
-  </si>
-  <si>
     <t>Standardangriffe</t>
   </si>
   <si>
@@ -361,6 +313,54 @@
   </si>
   <si>
     <t>Position 2</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/weltkarte.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/drachenkampf.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/ausruhen.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/standardangriffe.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/gegend_erkunden.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/gepaeck_betrachten.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/elemente_beschwoeren.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/elemente_der_erde.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/elemente_des_wassers.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/elemente_des_feuers.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/elemente_der_luft.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/fliegen.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/handwerk.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/tagebuch.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/jagen_angreifen.png</t>
+  </si>
+  <si>
+    <t>././Bilder/Buttons/pflanzen_sammeln.png</t>
   </si>
 </sst>
 </file>
@@ -480,16 +480,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -790,10 +781,10 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,13 +1129,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -1161,34 +1154,34 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -1209,10 +1202,10 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -1233,10 +1226,10 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F4" s="4">
         <v>2</v>
@@ -1260,7 +1253,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -1281,10 +1274,10 @@
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F6" s="13">
         <v>2</v>
@@ -1304,13 +1297,13 @@
         <v>42</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
@@ -1324,19 +1317,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -1350,17 +1343,17 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F9" s="10">
         <v>3</v>
@@ -1374,17 +1367,17 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F10" s="10">
         <v>3</v>
@@ -1398,17 +1391,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
@@ -1422,17 +1415,17 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F12" s="20">
         <v>3</v>
@@ -1446,19 +1439,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F13" s="19">
         <v>1</v>
@@ -1472,19 +1465,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F14" s="18">
         <v>1</v>
@@ -1498,19 +1491,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F15" s="21">
         <v>1</v>
@@ -1524,19 +1517,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
@@ -1550,19 +1543,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F17" s="11">
         <v>2</v>
@@ -1576,19 +1569,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F18" s="11">
         <v>2</v>
@@ -1602,19 +1595,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F19" s="11">
         <v>2</v>
@@ -1628,19 +1621,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F20" s="11">
         <v>2</v>
@@ -1654,19 +1647,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F21" s="19">
         <v>2</v>
@@ -1680,19 +1673,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1706,16 +1699,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
@@ -1736,13 +1729,13 @@
         <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F24" s="11">
         <v>1</v>
@@ -1804,14 +1797,14 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>36</v>
@@ -1822,14 +1815,14 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>35</v>
@@ -1840,17 +1833,17 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="12"/>
@@ -1858,19 +1851,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="12"/>
@@ -1878,19 +1871,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="12"/>
@@ -1898,17 +1891,17 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="12"/>
@@ -1916,19 +1909,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="12"/>
@@ -1936,17 +1929,17 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="12"/>
@@ -1954,17 +1947,17 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="12"/>
@@ -1972,17 +1965,17 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="12"/>
@@ -1990,17 +1983,17 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="12"/>
@@ -2008,17 +2001,17 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
@@ -2026,17 +2019,17 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="12"/>
@@ -2044,7 +2037,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -2060,17 +2053,17 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="12"/>
@@ -2078,17 +2071,17 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="12"/>
@@ -2096,17 +2089,17 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="12"/>
@@ -2114,17 +2107,17 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="12"/>
@@ -2132,17 +2125,17 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="12"/>
@@ -2150,17 +2143,17 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="12"/>
@@ -2168,7 +2161,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>

</xml_diff>